<commit_message>
battery and light level
</commit_message>
<xml_diff>
--- a/Design/pinmap.xlsx
+++ b/Design/pinmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Enes\SmartCar\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8D527C-9954-45E0-830F-37455F9F308F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{915975C0-D7C5-4D7D-987D-0598201821D9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{21C910A0-C4BA-4ED2-BDEF-B6A143B6589B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="69">
   <si>
     <t>İşlemci</t>
   </si>
@@ -201,30 +201,6 @@
     <t>OUT</t>
   </si>
   <si>
-    <t>Motor BL1</t>
-  </si>
-  <si>
-    <t>Motor BL2</t>
-  </si>
-  <si>
-    <t>Motor BR1</t>
-  </si>
-  <si>
-    <t>Motor BR2</t>
-  </si>
-  <si>
-    <t>Motor FL1</t>
-  </si>
-  <si>
-    <t>Motor FL2</t>
-  </si>
-  <si>
-    <t>Motor FR1</t>
-  </si>
-  <si>
-    <t>Motor FR2</t>
-  </si>
-  <si>
     <t>Wire1</t>
   </si>
   <si>
@@ -238,6 +214,33 @@
   </si>
   <si>
     <t>Buzzer</t>
+  </si>
+  <si>
+    <t>Motor L2</t>
+  </si>
+  <si>
+    <t>Motor L1</t>
+  </si>
+  <si>
+    <t>Motor R1</t>
+  </si>
+  <si>
+    <t>Motor R2</t>
+  </si>
+  <si>
+    <t>F ECHO</t>
+  </si>
+  <si>
+    <t>F TRIG</t>
+  </si>
+  <si>
+    <t>B TRIG</t>
+  </si>
+  <si>
+    <t>B ECHO</t>
+  </si>
+  <si>
+    <t>Back HL</t>
   </si>
 </sst>
 </file>
@@ -920,8 +923,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72128E52-0C0E-4B84-AC8D-E796181E61F1}">
   <dimension ref="B1:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,7 +1056,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
@@ -1069,7 +1072,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
@@ -1116,7 +1119,9 @@
       <c r="D12" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="5" t="s">
+        <v>60</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="23"/>
@@ -1130,7 +1135,9 @@
       <c r="D13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="22"/>
@@ -1144,7 +1151,9 @@
       <c r="D14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5" t="s">
+        <v>61</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="23"/>
@@ -1158,7 +1167,9 @@
       <c r="D15" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="22"/>
@@ -1284,9 +1295,7 @@
       <c r="D23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>55</v>
-      </c>
+      <c r="E23" s="7"/>
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="24"/>
@@ -1300,9 +1309,7 @@
       <c r="D24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="E24" s="9"/>
       <c r="F24" s="9"/>
       <c r="G24" s="9"/>
       <c r="H24" s="25"/>
@@ -1317,7 +1324,7 @@
         <v>23</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
@@ -1333,7 +1340,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="9"/>
@@ -1377,9 +1384,11 @@
         <v>25</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F29" s="7"/>
+        <v>65</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="G29" s="7"/>
       <c r="H29" s="24"/>
       <c r="I29" s="15"/>
@@ -1393,9 +1402,11 @@
         <v>26</v>
       </c>
       <c r="E30" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="F30" s="9"/>
+        <v>64</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>48</v>
+      </c>
       <c r="G30" s="9"/>
       <c r="H30" s="25"/>
       <c r="I30" s="16"/>
@@ -1445,9 +1456,11 @@
         <v>29</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F33" s="7"/>
+        <v>58</v>
+      </c>
+      <c r="F33" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="G33" s="7"/>
       <c r="H33" s="24"/>
       <c r="I33" s="15"/>
@@ -1461,9 +1474,11 @@
         <v>30</v>
       </c>
       <c r="E34" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F34" s="9"/>
+        <v>59</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="G34" s="9"/>
       <c r="H34" s="25"/>
       <c r="I34" s="16"/>
@@ -1477,9 +1492,11 @@
         <v>31</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="F35" s="7"/>
+        <v>57</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="G35" s="7"/>
       <c r="H35" s="24"/>
       <c r="I35" s="15"/>
@@ -1493,9 +1510,11 @@
         <v>32</v>
       </c>
       <c r="E36" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="F36" s="8"/>
+        <v>68</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="G36" s="8"/>
       <c r="H36" s="26"/>
       <c r="I36" s="17"/>
@@ -1508,9 +1527,7 @@
       <c r="D37" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E37" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="E37" s="7"/>
       <c r="F37" s="7"/>
       <c r="G37" s="7"/>
       <c r="H37" s="24"/>
@@ -1524,9 +1541,7 @@
       <c r="D38" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E38" s="9" t="s">
-        <v>61</v>
-      </c>
+      <c r="E38" s="9"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9"/>
       <c r="H38" s="25"/>
@@ -1541,9 +1556,11 @@
         <v>12</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F39" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="G39" s="7"/>
       <c r="H39" s="24"/>
       <c r="I39" s="15"/>
@@ -1556,8 +1573,12 @@
       <c r="D40" s="18">
         <v>13</v>
       </c>
-      <c r="E40" s="19"/>
-      <c r="F40" s="19"/>
+      <c r="E40" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>48</v>
+      </c>
       <c r="G40" s="19"/>
       <c r="H40" s="27"/>
       <c r="I40" s="20"/>

</xml_diff>